<commit_message>
update excel file project details
</commit_message>
<xml_diff>
--- a/project details.xlsx
+++ b/project details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danico.balane\source\repos\ASMK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3B817B3-4EDC-42EA-BB22-D46E1ADDE75B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AD549C93-4C4F-4D4E-BF44-B8A1F26C942B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9564F456-4196-4474-B685-CD4E9B889504}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Login</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>export/generate</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>k</t>
   </si>
 </sst>
 </file>
@@ -85,7 +91,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,6 +101,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -110,6 +122,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -209,11 +233,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -241,14 +268,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -564,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9532E5F3-6DD6-4596-B2D6-EF30FC671D30}">
-  <dimension ref="B3:F11"/>
+  <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,104 +617,140 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="17"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="3" t="s">
+      <c r="G5" s="15"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="13" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="3" t="s">
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="10"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="12" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="3"/>
+      <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="12" t="s">
+      <c r="E8" s="4"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+      <c r="C9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="10"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="3"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="8"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="9"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="9"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
importing of excel file
</commit_message>
<xml_diff>
--- a/project details.xlsx
+++ b/project details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danico.balane\source\repos\ASMK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AD549C93-4C4F-4D4E-BF44-B8A1F26C942B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2710E3AD-7437-4495-9B9A-FE8E5AE9D9E3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9564F456-4196-4474-B685-CD4E9B889504}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Login</t>
   </si>
@@ -76,16 +76,47 @@
   </si>
   <si>
     <t>k</t>
+  </si>
+  <si>
+    <t>DATE:</t>
+  </si>
+  <si>
+    <t>2k</t>
+  </si>
+  <si>
+    <t>3k</t>
+  </si>
+  <si>
+    <t>5k</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total Pending</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,7 +166,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -229,11 +260,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -285,6 +388,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9532E5F3-6DD6-4596-B2D6-EF30FC671D30}">
-  <dimension ref="B2:G11"/>
+  <dimension ref="A2:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,7 +765,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="17"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16" t="s">
@@ -626,7 +774,7 @@
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
     </row>
-    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -646,7 +794,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
@@ -664,7 +812,7 @@
       </c>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
@@ -682,7 +830,7 @@
       </c>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
         <v>5</v>
@@ -696,7 +844,7 @@
       </c>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
         <v>6</v>
@@ -708,19 +856,19 @@
       <c r="F7" s="11"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="11"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="13" t="s">
         <v>11</v>
@@ -732,7 +880,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12" t="s">
@@ -742,7 +890,7 @@
       <c r="F10" s="11"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8" t="s">
@@ -752,7 +900,92 @@
       <c r="F11" s="10"/>
       <c r="G11" s="15"/>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="19">
+        <v>43328</v>
+      </c>
+      <c r="C12" s="19">
+        <v>43336</v>
+      </c>
+      <c r="D12" s="20">
+        <v>43343</v>
+      </c>
+      <c r="E12" s="19">
+        <v>43328</v>
+      </c>
+      <c r="F12" s="20">
+        <v>43343</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="21"/>
+      <c r="C14" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="23">
+        <v>43328</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="25">
+        <v>1</v>
+      </c>
+      <c r="E15" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="23">
+        <v>43336</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="30"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="26">
+        <v>43343</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="27"/>
+      <c r="E17" s="31"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="28"/>
+      <c r="C18" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="5">
+        <f>SUM(D15:D17)</f>
+        <v>1</v>
+      </c>
+      <c r="E18" s="32">
+        <f>SUM(E15:E17)</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Guest View and file searching
</commit_message>
<xml_diff>
--- a/project details.xlsx
+++ b/project details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danico.balane\source\repos\ASMK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2710E3AD-7437-4495-9B9A-FE8E5AE9D9E3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6AA19D4C-FE9D-4142-8FED-0744D186BEB6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9564F456-4196-4474-B685-CD4E9B889504}"/>
   </bookViews>
@@ -122,7 +122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,12 +138,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -374,16 +368,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -751,7 +739,7 @@
   <dimension ref="A2:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,13 +754,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="17"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
@@ -810,7 +798,7 @@
       <c r="F4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="15"/>
+      <c r="G4" s="13"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -825,10 +813,10 @@
       <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
@@ -839,10 +827,10 @@
         <v>5</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
@@ -854,41 +842,41 @@
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="15"/>
+      <c r="G7" s="13"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="16" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="15"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="15"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="15"/>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9"/>
@@ -898,88 +886,88 @@
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="15"/>
+      <c r="G11" s="13"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="17">
         <v>43328</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="17">
         <v>43336</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="18">
         <v>43343</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E12" s="17">
         <v>43328</v>
       </c>
-      <c r="F12" s="20">
+      <c r="F12" s="18">
         <v>43343</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="21"/>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="23">
+      <c r="B15" s="21">
         <v>43328</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="23">
         <v>1</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="23">
+      <c r="B16" s="21">
         <v>43336</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="30"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="28"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="26">
+      <c r="B17" s="24">
         <v>43343</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="31"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="29"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="27" t="s">
+      <c r="B18" s="26"/>
+      <c r="C18" s="25" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="5">
         <f>SUM(D15:D17)</f>
         <v>1</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="30">
         <f>SUM(E15:E17)</f>
         <v>1</v>
       </c>

</xml_diff>